<commit_message>
Update src allocation. (Kaii)
</commit_message>
<xml_diff>
--- a/PCB/02 Plans & Actuals/2.2_WBS & Sprint plan/SeeNowDo_Task_assignment_20150913.xlsx
+++ b/PCB/02 Plans & Actuals/2.2_WBS & Sprint plan/SeeNowDo_Task_assignment_20150913.xlsx
@@ -11,14 +11,14 @@
     <sheet name="Scoure Code" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Task List'!$F$2:$H$46</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Task List'!$F$2:$H$47</definedName>
   </definedNames>
   <calcPr calcId="145621" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="296">
   <si>
     <t>User Story</t>
   </si>
@@ -722,9 +722,6 @@
     <t>│  │      login2.html</t>
   </si>
   <si>
-    <t>│  │      success story main - 副本.html</t>
-  </si>
-  <si>
     <t>│  │      successstory.html</t>
   </si>
   <si>
@@ -909,6 +906,9 @@
   </si>
   <si>
     <t>V, Kaii</t>
+  </si>
+  <si>
+    <t>Clay</t>
   </si>
 </sst>
 </file>
@@ -1054,7 +1054,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1093,6 +1093,14 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1394,7 +1402,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H46"/>
+  <dimension ref="B2:H47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1464,37 +1472,39 @@
       <c r="E4" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="12"/>
+      <c r="F4" s="12" t="s">
+        <v>6</v>
+      </c>
       <c r="G4" s="12"/>
       <c r="H4" s="13">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" s="7"/>
       <c r="C5" s="8"/>
       <c r="D5" s="11">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="F5" s="12" t="s">
         <v>10</v>
       </c>
       <c r="G5" s="12"/>
       <c r="H5" s="13">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" s="7"/>
       <c r="C6" s="8"/>
       <c r="D6" s="11">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F6" s="12" t="s">
         <v>10</v>
@@ -1505,143 +1515,143 @@
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="5">
-        <v>2</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>12</v>
-      </c>
+      <c r="B7" s="7"/>
+      <c r="C7" s="8"/>
       <c r="D7" s="11">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="G7" s="12"/>
       <c r="H7" s="13">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="7"/>
-      <c r="C8" s="8"/>
+      <c r="B8" s="5">
+        <v>2</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="D8" s="11">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="G8" s="12"/>
       <c r="H8" s="13">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="7"/>
       <c r="C9" s="8"/>
       <c r="D9" s="11">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="G9" s="12"/>
       <c r="H9" s="13">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="9"/>
-      <c r="C10" s="10"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="8"/>
       <c r="D10" s="11">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="G10" s="12"/>
       <c r="H10" s="13">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="7">
-        <v>3</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>21</v>
-      </c>
+      <c r="B11" s="9"/>
+      <c r="C11" s="10"/>
       <c r="D11" s="11">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G11" s="12"/>
       <c r="H11" s="13">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="7"/>
-      <c r="C12" s="8"/>
+      <c r="B12" s="7">
+        <v>3</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>21</v>
+      </c>
       <c r="D12" s="11">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="F12" s="12"/>
+        <v>22</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>6</v>
+      </c>
       <c r="G12" s="12"/>
       <c r="H12" s="13">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="7"/>
       <c r="C13" s="8"/>
       <c r="D13" s="11">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="F13" s="12"/>
+        <v>23</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>42</v>
+      </c>
       <c r="G13" s="12"/>
       <c r="H13" s="13">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="5">
-        <v>4</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="B14" s="7"/>
+      <c r="C14" s="8"/>
       <c r="D14" s="11">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>6</v>
+        <v>42</v>
       </c>
       <c r="G14" s="12"/>
       <c r="H14" s="13">
@@ -1649,16 +1659,20 @@
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="9"/>
-      <c r="C15" s="10"/>
+      <c r="B15" s="5">
+        <v>4</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>25</v>
+      </c>
       <c r="D15" s="11">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="G15" s="12"/>
       <c r="H15" s="13">
@@ -1666,58 +1680,58 @@
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="7">
-        <v>5</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>28</v>
-      </c>
+      <c r="B16" s="9"/>
+      <c r="C16" s="10"/>
       <c r="D16" s="11">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="G16" s="12"/>
       <c r="H16" s="13">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="7"/>
-      <c r="C17" s="8"/>
+      <c r="B17" s="7">
+        <v>5</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>28</v>
+      </c>
       <c r="D17" s="11">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F17" s="12" t="s">
         <v>40</v>
       </c>
       <c r="G17" s="12"/>
       <c r="H17" s="13">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="7"/>
       <c r="C18" s="8"/>
       <c r="D18" s="11">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G18" s="12"/>
       <c r="H18" s="13">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
@@ -1730,38 +1744,38 @@
         <v>33</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G19" s="12"/>
       <c r="H19" s="13">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="7"/>
       <c r="C20" s="8"/>
       <c r="D20" s="11">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G20" s="12"/>
       <c r="H20" s="13">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="7"/>
       <c r="C21" s="8"/>
       <c r="D21" s="11">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F21" s="12" t="s">
         <v>42</v>
@@ -1775,13 +1789,13 @@
       <c r="B22" s="7"/>
       <c r="C22" s="8"/>
       <c r="D22" s="11">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F22" s="12" t="s">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="G22" s="12"/>
       <c r="H22" s="13">
@@ -1792,30 +1806,30 @@
       <c r="B23" s="7"/>
       <c r="C23" s="8"/>
       <c r="D23" s="11">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="F23" s="12" t="s">
         <v>16</v>
       </c>
       <c r="G23" s="12"/>
       <c r="H23" s="13">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="7"/>
       <c r="C24" s="8"/>
       <c r="D24" s="11">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E24" s="12" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="F24" s="12" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="G24" s="12"/>
       <c r="H24" s="13">
@@ -1823,71 +1837,69 @@
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B25" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D25" s="11">
-        <v>11</v>
-      </c>
-      <c r="E25" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="F25" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="G25" s="12"/>
-      <c r="H25" s="13">
-        <v>2</v>
+      <c r="B25" s="7"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="20">
+        <v>58</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G25" s="6"/>
+      <c r="H25" s="21">
+        <v>3</v>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B26" s="7"/>
-      <c r="C26" s="8"/>
+      <c r="B26" s="5">
+        <v>6</v>
+      </c>
+      <c r="C26" s="6"/>
       <c r="D26" s="11">
-        <v>12</v>
+        <v>61</v>
       </c>
       <c r="E26" s="12" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="F26" s="12" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G26" s="12"/>
       <c r="H26" s="13">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27" s="7"/>
       <c r="C27" s="8"/>
       <c r="D27" s="11">
-        <v>12</v>
+        <v>62</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="F27" s="12" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="G27" s="12"/>
       <c r="H27" s="13">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B28" s="7"/>
-      <c r="C28" s="8"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="10"/>
       <c r="D28" s="11">
-        <v>13</v>
+        <v>63</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="F28" s="12" t="s">
-        <v>41</v>
+        <v>10</v>
       </c>
       <c r="G28" s="12"/>
       <c r="H28" s="13">
@@ -1895,101 +1907,105 @@
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B29" s="7"/>
-      <c r="C29" s="8"/>
+      <c r="B29" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>30</v>
+      </c>
       <c r="D29" s="11">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E29" s="12" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F29" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G29" s="12"/>
       <c r="H29" s="13">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B30" s="7"/>
       <c r="C30" s="8"/>
       <c r="D30" s="11">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F30" s="12" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="G30" s="12"/>
       <c r="H30" s="13">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B31" s="7"/>
       <c r="C31" s="8"/>
       <c r="D31" s="11">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="E31" s="12" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F31" s="12" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="G31" s="12"/>
       <c r="H31" s="13">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B32" s="7"/>
       <c r="C32" s="8"/>
       <c r="D32" s="11">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="E32" s="12" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F32" s="12" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="G32" s="12"/>
       <c r="H32" s="13">
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B33" s="7"/>
       <c r="C33" s="8"/>
       <c r="D33" s="11">
-        <v>61</v>
+        <v>13</v>
       </c>
       <c r="E33" s="12" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F33" s="12" t="s">
         <v>42</v>
       </c>
       <c r="G33" s="12"/>
       <c r="H33" s="13">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B34" s="7"/>
       <c r="C34" s="8"/>
       <c r="D34" s="11">
-        <v>62</v>
+        <v>21</v>
       </c>
       <c r="E34" s="12" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="F34" s="12" t="s">
-        <v>10</v>
+        <v>47</v>
       </c>
       <c r="G34" s="12"/>
       <c r="H34" s="13">
@@ -1997,68 +2013,68 @@
       </c>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B35" s="9"/>
-      <c r="C35" s="10"/>
+      <c r="B35" s="7"/>
+      <c r="C35" s="8"/>
       <c r="D35" s="11">
-        <v>63</v>
+        <v>22</v>
       </c>
       <c r="E35" s="12" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="F35" s="12" t="s">
-        <v>10</v>
+        <v>47</v>
       </c>
       <c r="G35" s="12"/>
       <c r="H35" s="13">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B36" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C36" s="8" t="s">
-        <v>32</v>
-      </c>
+      <c r="B36" s="9"/>
+      <c r="C36" s="10"/>
       <c r="D36" s="11">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="E36" s="12" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="F36" s="12" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="G36" s="12"/>
       <c r="H36" s="13">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B37" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D37" s="22">
+        <v>1</v>
+      </c>
+      <c r="E37" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="F37" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="G37" s="10"/>
+      <c r="H37" s="23">
         <v>4</v>
-      </c>
-    </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B37" s="7"/>
-      <c r="C37" s="8"/>
-      <c r="D37" s="11">
-        <v>2</v>
-      </c>
-      <c r="E37" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="F37" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="G37" s="12"/>
-      <c r="H37" s="13">
-        <v>1</v>
       </c>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B38" s="7"/>
       <c r="C38" s="8"/>
       <c r="D38" s="11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E38" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F38" s="12" t="s">
         <v>40</v>
@@ -2072,13 +2088,13 @@
       <c r="B39" s="7"/>
       <c r="C39" s="8"/>
       <c r="D39" s="11">
-        <v>91</v>
+        <v>3</v>
       </c>
       <c r="E39" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F39" s="12" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="G39" s="12"/>
       <c r="H39" s="13">
@@ -2089,10 +2105,10 @@
       <c r="B40" s="7"/>
       <c r="C40" s="8"/>
       <c r="D40" s="11">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E40" s="12" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F40" s="12" t="s">
         <v>54</v>
@@ -2106,10 +2122,10 @@
       <c r="B41" s="7"/>
       <c r="C41" s="8"/>
       <c r="D41" s="11">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E41" s="12" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F41" s="12" t="s">
         <v>54</v>
@@ -2123,10 +2139,10 @@
       <c r="B42" s="7"/>
       <c r="C42" s="8"/>
       <c r="D42" s="11">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E42" s="12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F42" s="12" t="s">
         <v>54</v>
@@ -2140,10 +2156,10 @@
       <c r="B43" s="7"/>
       <c r="C43" s="8"/>
       <c r="D43" s="11">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E43" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F43" s="12" t="s">
         <v>54</v>
@@ -2157,41 +2173,41 @@
       <c r="B44" s="7"/>
       <c r="C44" s="8"/>
       <c r="D44" s="11">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E44" s="12" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F44" s="12" t="s">
         <v>54</v>
       </c>
       <c r="G44" s="12"/>
       <c r="H44" s="13">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B45" s="7"/>
       <c r="C45" s="8"/>
       <c r="D45" s="11">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E45" s="12" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F45" s="12" t="s">
         <v>54</v>
       </c>
       <c r="G45" s="12"/>
       <c r="H45" s="13">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="46" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B46" s="9"/>
-      <c r="C46" s="10"/>
+      <c r="B46" s="7"/>
+      <c r="C46" s="8"/>
       <c r="D46" s="11">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E46" s="12" t="s">
         <v>62</v>
@@ -2201,11 +2217,28 @@
       </c>
       <c r="G46" s="12"/>
       <c r="H46" s="13">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B47" s="9"/>
+      <c r="C47" s="10"/>
+      <c r="D47" s="11">
+        <v>98</v>
+      </c>
+      <c r="E47" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="F47" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="G47" s="12"/>
+      <c r="H47" s="13">
         <v>2</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="F2:H46"/>
+  <autoFilter ref="F2:H47"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -2213,9 +2246,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:AG258"/>
+  <dimension ref="B1:AG257"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A242" workbookViewId="0">
+      <selection activeCell="AG270" sqref="AG270"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.7109375" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2423,7 +2458,7 @@
         <v>94</v>
       </c>
       <c r="E34" s="14" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="AG34" s="18"/>
     </row>
@@ -2581,7 +2616,9 @@
       <c r="B60" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="AG60" s="18"/>
+      <c r="AG60" s="18" t="s">
+        <v>295</v>
+      </c>
     </row>
     <row r="61" spans="2:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B61" s="15" t="s">
@@ -2968,7 +3005,7 @@
         <v>94</v>
       </c>
       <c r="E77" s="14" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="AG77" s="18"/>
     </row>
@@ -3406,7 +3443,7 @@
     </row>
     <row r="148" spans="2:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B148" s="15" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="AG148" s="18"/>
     </row>
@@ -3606,7 +3643,9 @@
       <c r="B181" s="15" t="s">
         <v>230</v>
       </c>
-      <c r="AG181" s="18"/>
+      <c r="AG181" s="18" t="s">
+        <v>295</v>
+      </c>
     </row>
     <row r="182" spans="2:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B182" s="15" t="s">
@@ -3640,13 +3679,13 @@
     </row>
     <row r="187" spans="2:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B187" s="15" t="s">
-        <v>236</v>
+        <v>69</v>
       </c>
       <c r="AG187" s="18"/>
     </row>
     <row r="188" spans="2:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B188" s="15" t="s">
-        <v>69</v>
+        <v>236</v>
       </c>
       <c r="AG188" s="18"/>
     </row>
@@ -3786,29 +3825,35 @@
       <c r="B211" s="15" t="s">
         <v>259</v>
       </c>
-      <c r="AG211" s="18"/>
+      <c r="AG211" s="18" t="s">
+        <v>295</v>
+      </c>
     </row>
     <row r="212" spans="2:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B212" s="15" t="s">
         <v>260</v>
       </c>
-      <c r="AG212" s="18"/>
+      <c r="AG212" s="18" t="s">
+        <v>295</v>
+      </c>
     </row>
     <row r="213" spans="2:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B213" s="15" t="s">
         <v>261</v>
       </c>
-      <c r="AG213" s="18"/>
+      <c r="AG213" s="18" t="s">
+        <v>295</v>
+      </c>
     </row>
     <row r="214" spans="2:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B214" s="15" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="AG214" s="18"/>
     </row>
     <row r="215" spans="2:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B215" s="15" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
       <c r="AG215" s="18"/>
     </row>
@@ -3826,13 +3871,13 @@
     </row>
     <row r="218" spans="2:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B218" s="15" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="AG218" s="18"/>
     </row>
     <row r="219" spans="2:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B219" s="15" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="AG219" s="18"/>
     </row>
@@ -3850,13 +3895,13 @@
     </row>
     <row r="222" spans="2:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B222" s="15" t="s">
-        <v>268</v>
+        <v>254</v>
       </c>
       <c r="AG222" s="18"/>
     </row>
     <row r="223" spans="2:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B223" s="15" t="s">
-        <v>255</v>
+        <v>268</v>
       </c>
       <c r="AG223" s="18"/>
     </row>
@@ -3870,17 +3915,19 @@
       <c r="B225" s="15" t="s">
         <v>270</v>
       </c>
-      <c r="AG225" s="18"/>
+      <c r="AG225" s="18" t="s">
+        <v>295</v>
+      </c>
     </row>
     <row r="226" spans="2:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B226" s="15" t="s">
-        <v>271</v>
+        <v>254</v>
       </c>
       <c r="AG226" s="18"/>
     </row>
     <row r="227" spans="2:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B227" s="15" t="s">
-        <v>255</v>
+        <v>271</v>
       </c>
       <c r="AG227" s="18"/>
     </row>
@@ -3888,14 +3935,16 @@
       <c r="B228" s="15" t="s">
         <v>272</v>
       </c>
-      <c r="AG228" s="18"/>
+      <c r="AG228" s="18" t="s">
+        <v>294</v>
+      </c>
     </row>
     <row r="229" spans="2:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B229" s="15" t="s">
         <v>273</v>
       </c>
       <c r="AG229" s="18" t="s">
-        <v>295</v>
+        <v>40</v>
       </c>
     </row>
     <row r="230" spans="2:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3903,7 +3952,7 @@
         <v>274</v>
       </c>
       <c r="AG230" s="18" t="s">
-        <v>40</v>
+        <v>295</v>
       </c>
     </row>
     <row r="231" spans="2:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3927,7 +3976,7 @@
         <v>277</v>
       </c>
       <c r="AG233" s="18" t="s">
-        <v>40</v>
+        <v>295</v>
       </c>
     </row>
     <row r="234" spans="2:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3936,11 +3985,11 @@
       </c>
       <c r="AG234" s="18"/>
     </row>
-    <row r="235" spans="2:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B235" s="15" t="s">
+    <row r="235" spans="2:33" s="16" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B235" s="17" t="s">
         <v>279</v>
       </c>
-      <c r="AG235" s="18"/>
+      <c r="AG235" s="19"/>
     </row>
     <row r="236" spans="2:33" s="16" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B236" s="17" t="s">
@@ -3956,43 +4005,43 @@
     </row>
     <row r="238" spans="2:33" s="16" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B238" s="17" t="s">
-        <v>282</v>
+        <v>77</v>
       </c>
       <c r="AG238" s="19"/>
     </row>
     <row r="239" spans="2:33" s="16" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B239" s="17" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="AG239" s="19"/>
     </row>
     <row r="240" spans="2:33" s="16" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B240" s="17" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="AG240" s="19"/>
     </row>
     <row r="241" spans="2:33" s="16" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B241" s="17" t="s">
-        <v>93</v>
+        <v>292</v>
       </c>
       <c r="AG241" s="19"/>
     </row>
     <row r="242" spans="2:33" s="16" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B242" s="17" t="s">
-        <v>293</v>
+        <v>116</v>
       </c>
       <c r="AG242" s="19"/>
     </row>
-    <row r="243" spans="2:33" s="16" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B243" s="17" t="s">
-        <v>116</v>
-      </c>
-      <c r="AG243" s="19"/>
+    <row r="243" spans="2:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B243" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="AG243" s="18"/>
     </row>
     <row r="244" spans="2:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B244" s="15" t="s">
-        <v>117</v>
+        <v>282</v>
       </c>
       <c r="AG244" s="18"/>
     </row>
@@ -4014,27 +4063,27 @@
       </c>
       <c r="AG247" s="18"/>
     </row>
-    <row r="248" spans="2:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B248" s="15" t="s">
-        <v>286</v>
-      </c>
-      <c r="AG248" s="18"/>
+    <row r="248" spans="2:33" s="16" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B248" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="AG248" s="19"/>
     </row>
     <row r="249" spans="2:33" s="16" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B249" s="17" t="s">
-        <v>69</v>
+        <v>201</v>
       </c>
       <c r="AG249" s="19"/>
     </row>
     <row r="250" spans="2:33" s="16" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B250" s="17" t="s">
-        <v>201</v>
+        <v>292</v>
       </c>
       <c r="AG250" s="19"/>
     </row>
     <row r="251" spans="2:33" s="16" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B251" s="17" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="AG251" s="19"/>
     </row>
@@ -4058,27 +4107,21 @@
     </row>
     <row r="255" spans="2:33" s="16" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B255" s="17" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="AG255" s="19"/>
     </row>
     <row r="256" spans="2:33" s="16" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B256" s="17" t="s">
-        <v>294</v>
+        <v>278</v>
       </c>
       <c r="AG256" s="19"/>
     </row>
     <row r="257" spans="2:33" s="16" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B257" s="17" t="s">
-        <v>279</v>
+        <v>290</v>
       </c>
       <c r="AG257" s="19"/>
-    </row>
-    <row r="258" spans="2:33" s="16" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B258" s="17" t="s">
-        <v>291</v>
-      </c>
-      <c r="AG258" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>